<commit_message>
final corrections and accuracy fix
</commit_message>
<xml_diff>
--- a/df_both_seasons_away.xlsx
+++ b/df_both_seasons_away.xlsx
@@ -455,22 +455,22 @@
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.4</v>
+        <v>-0.5</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -500,22 +500,22 @@
         <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="M3" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="4">
@@ -545,19 +545,19 @@
         <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.4</v>
+        <v>-0.6</v>
       </c>
       <c r="M4" t="n">
         <v>1.1</v>
@@ -578,34 +578,34 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>FC Koln</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G5" t="n">
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.9</v>
+        <v>-0.7</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="6">
@@ -635,22 +635,22 @@
         <v>2</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="M6" t="n">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="7">
@@ -668,31 +668,31 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Schalke 04</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.6</v>
+        <v>-1.1</v>
       </c>
       <c r="M7" t="n">
         <v>1</v>
@@ -713,22 +713,22 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>FC Koln</t>
+          <t>Schalke 04</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G8" t="n">
         <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -740,7 +740,7 @@
         <v>-0.6</v>
       </c>
       <c r="M8" t="n">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="9">
@@ -773,7 +773,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -815,22 +815,22 @@
         <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.2</v>
+        <v>-0.3</v>
       </c>
       <c r="M10" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="11">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" t="n">
         <v>6</v>
@@ -947,7 +947,7 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H13" t="n">
         <v>5</v>
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
         <v>11</v>
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H16" t="n">
         <v>5</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B23" t="n">
         <v>14</v>
@@ -1388,39 +1388,39 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>FC Koln</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G23" t="n">
         <v>1</v>
       </c>
       <c r="H23" t="n">
+        <v>14</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J23" t="n">
         <v>5</v>
       </c>
-      <c r="I23" t="n">
-        <v>2</v>
-      </c>
-      <c r="J23" t="n">
-        <v>2</v>
-      </c>
       <c r="K23" t="n">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="L23" t="n">
-        <v>0.8</v>
+        <v>-0.9</v>
       </c>
       <c r="M23" t="n">
-        <v>2.3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B24" t="n">
         <v>14</v>
@@ -1433,39 +1433,39 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Hertha</t>
+          <t>FC Koln</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H24" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I24" t="n">
         <v>2</v>
       </c>
       <c r="J24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.7</v>
+        <v>0.8</v>
       </c>
       <c r="M24" t="n">
-        <v>1.1</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B25" t="n">
         <v>14</v>
@@ -1478,34 +1478,34 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>Hertha</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G25" t="n">
         <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I25" t="n">
         <v>2</v>
       </c>
       <c r="J25" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="L25" t="n">
-        <v>-0.9</v>
+        <v>-0.7</v>
       </c>
       <c r="M25" t="n">
-        <v>1.5</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="26">
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H28" t="n">
         <v>8</v>
@@ -1712,7 +1712,7 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30" t="n">
         <v>7</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B35" t="n">
         <v>30</v>
@@ -1920,39 +1920,39 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>FC Koln</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H35" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I35" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35" t="n">
-        <v>-1.8</v>
+        <v>1.3</v>
       </c>
       <c r="M35" t="n">
-        <v>0.6</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B36" t="n">
         <v>30</v>
@@ -1965,34 +1965,34 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>FC Koln</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H36" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I36" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J36" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>1.3</v>
+        <v>-1.8</v>
       </c>
       <c r="M36" t="n">
-        <v>2.7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="37">
@@ -2109,7 +2109,7 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H39" t="n">
         <v>4</v>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B51" t="n">
         <v>5</v>
@@ -2640,39 +2640,39 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Hannover</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G51" t="n">
         <v>1</v>
       </c>
       <c r="H51" t="n">
+        <v>3</v>
+      </c>
+      <c r="I51" t="n">
         <v>6</v>
       </c>
-      <c r="I51" t="n">
-        <v>1</v>
-      </c>
       <c r="J51" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="K51" t="n">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="L51" t="n">
-        <v>-0.6</v>
+        <v>-0.5</v>
       </c>
       <c r="M51" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B52" t="n">
         <v>5</v>
@@ -2685,34 +2685,34 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Hannover</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G52" t="n">
         <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I52" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J52" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="K52" t="n">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="L52" t="n">
-        <v>-0.5</v>
+        <v>-0.6</v>
       </c>
       <c r="M52" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="53">
@@ -2739,7 +2739,7 @@
         </is>
       </c>
       <c r="G53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H53" t="n">
         <v>2</v>
@@ -2829,7 +2829,7 @@
         </is>
       </c>
       <c r="G55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H55" t="n">
         <v>3</v>
@@ -2919,7 +2919,7 @@
         </is>
       </c>
       <c r="G57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H57" t="n">
         <v>5</v>
@@ -2964,7 +2964,7 @@
         </is>
       </c>
       <c r="G58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
         <v>3</v>
@@ -3369,7 +3369,7 @@
         </is>
       </c>
       <c r="G67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H67" t="n">
         <v>6</v>
@@ -3684,7 +3684,7 @@
         </is>
       </c>
       <c r="G74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H74" t="n">
         <v>7</v>
@@ -3842,7 +3842,7 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B78" t="n">
         <v>11</v>
@@ -3855,39 +3855,39 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>M'gladbach</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H78" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I78" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J78" t="n">
+        <v>2</v>
+      </c>
+      <c r="K78" t="n">
         <v>-2</v>
       </c>
-      <c r="K78" t="n">
-        <v>2</v>
-      </c>
       <c r="L78" t="n">
-        <v>1.3</v>
+        <v>-0.4</v>
       </c>
       <c r="M78" t="n">
-        <v>2.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B79" t="n">
         <v>11</v>
@@ -3900,34 +3900,34 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>M'gladbach</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H79" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I79" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J79" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="K79" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="L79" t="n">
-        <v>-0.4</v>
+        <v>1.3</v>
       </c>
       <c r="M79" t="n">
-        <v>1.5</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="80">
@@ -4179,7 +4179,7 @@
         </is>
       </c>
       <c r="G85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H85" t="n">
         <v>7</v>
@@ -4269,7 +4269,7 @@
         </is>
       </c>
       <c r="G87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H87" t="n">
         <v>5</v>
@@ -4292,7 +4292,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B88" t="n">
         <v>28</v>
@@ -4305,39 +4305,39 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I88" t="n">
         <v>5</v>
       </c>
       <c r="J88" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="K88" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L88" t="n">
-        <v>1.2</v>
+        <v>-0.2</v>
       </c>
       <c r="M88" t="n">
-        <v>2.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B89" t="n">
         <v>28</v>
@@ -4350,34 +4350,34 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="G89" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H89" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I89" t="n">
         <v>5</v>
       </c>
       <c r="J89" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="K89" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L89" t="n">
-        <v>-0.2</v>
+        <v>1.2</v>
       </c>
       <c r="M89" t="n">
-        <v>1.5</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="90">
@@ -4404,7 +4404,7 @@
         </is>
       </c>
       <c r="G90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H90" t="n">
         <v>4</v>
@@ -4449,7 +4449,7 @@
         </is>
       </c>
       <c r="G91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H91" t="n">
         <v>5</v>
@@ -4584,7 +4584,7 @@
         </is>
       </c>
       <c r="G94" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H94" t="n">
         <v>4</v>
@@ -4854,7 +4854,7 @@
         </is>
       </c>
       <c r="G100" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H100" t="n">
         <v>4</v>
@@ -5034,7 +5034,7 @@
         </is>
       </c>
       <c r="G104" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H104" t="n">
         <v>1</v>
@@ -5102,7 +5102,7 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B106" t="n">
         <v>14</v>
@@ -5115,39 +5115,39 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G106" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H106" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I106" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J106" t="n">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="K106" t="n">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="L106" t="n">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="M106" t="n">
-        <v>2.6</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B107" t="n">
         <v>14</v>
@@ -5160,34 +5160,34 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="G107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H107" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I107" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J107" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="K107" t="n">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="L107" t="n">
-        <v>-0.2</v>
+        <v>1</v>
       </c>
       <c r="M107" t="n">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="108">
@@ -5304,7 +5304,7 @@
         </is>
       </c>
       <c r="G110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H110" t="n">
         <v>6</v>
@@ -5484,7 +5484,7 @@
         </is>
       </c>
       <c r="G114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H114" t="n">
         <v>5</v>
@@ -6067,7 +6067,7 @@
         </is>
       </c>
       <c r="G127" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H127" t="n">
         <v>4</v>
@@ -6112,7 +6112,7 @@
         </is>
       </c>
       <c r="G128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H128" t="n">
         <v>4</v>
@@ -6425,7 +6425,7 @@
         </is>
       </c>
       <c r="G135" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H135" t="n">
         <v>5</v>
@@ -6515,7 +6515,7 @@
         </is>
       </c>
       <c r="G137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H137" t="n">
         <v>2</v>
@@ -6718,7 +6718,7 @@
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B142" t="n">
         <v>24</v>
@@ -6731,39 +6731,39 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Fortuna Dusseldorf</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G142" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H142" t="n">
+        <v>3</v>
+      </c>
+      <c r="I142" t="n">
         <v>6</v>
       </c>
-      <c r="I142" t="n">
-        <v>7</v>
-      </c>
       <c r="J142" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="K142" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="L142" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="M142" t="n">
         <v>1.3</v>
-      </c>
-      <c r="M142" t="n">
-        <v>2.7</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B143" t="n">
         <v>24</v>
@@ -6776,22 +6776,22 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Paderborn</t>
+          <t>Fortuna Dusseldorf</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="G143" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H143" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I143" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J143" t="n">
         <v>-2</v>
@@ -6800,15 +6800,15 @@
         <v>2</v>
       </c>
       <c r="L143" t="n">
-        <v>-0.9</v>
+        <v>1.3</v>
       </c>
       <c r="M143" t="n">
-        <v>1.1</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B144" t="n">
         <v>24</v>
@@ -6821,34 +6821,34 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Paderborn</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G144" t="n">
         <v>1</v>
       </c>
       <c r="H144" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I144" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J144" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="K144" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="L144" t="n">
-        <v>-0.2</v>
+        <v>-0.9</v>
       </c>
       <c r="M144" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="145">
@@ -6920,7 +6920,7 @@
         </is>
       </c>
       <c r="G146" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H146" t="n">
         <v>2</v>
@@ -7010,7 +7010,7 @@
         </is>
       </c>
       <c r="G148" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H148" t="n">
         <v>2</v>
@@ -7235,7 +7235,7 @@
         </is>
       </c>
       <c r="G153" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H153" t="n">
         <v>4</v>
@@ -7415,7 +7415,7 @@
         </is>
       </c>
       <c r="G157" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H157" t="n">
         <v>5</v>
@@ -7638,7 +7638,7 @@
         </is>
       </c>
       <c r="G162" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H162" t="n">
         <v>2</v>
@@ -7771,7 +7771,7 @@
         </is>
       </c>
       <c r="G165" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H165" t="n">
         <v>3</v>
@@ -7816,7 +7816,7 @@
         </is>
       </c>
       <c r="G166" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H166" t="n">
         <v>9</v>
@@ -7951,7 +7951,7 @@
         </is>
       </c>
       <c r="G169" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H169" t="n">
         <v>14</v>
@@ -8041,7 +8041,7 @@
         </is>
       </c>
       <c r="G171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H171" t="n">
         <v>3</v>
@@ -8086,7 +8086,7 @@
         </is>
       </c>
       <c r="G172" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H172" t="n">
         <v>3</v>
@@ -8244,7 +8244,7 @@
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B176" t="n">
         <v>10</v>
@@ -8257,39 +8257,39 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>M'gladbach</t>
+          <t>Ein Frankfurt</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G176" t="n">
         <v>1</v>
       </c>
       <c r="H176" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I176" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J176" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K176" t="n">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="L176" t="n">
-        <v>-1.8</v>
+        <v>-0.1</v>
       </c>
       <c r="M176" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B177" t="n">
         <v>10</v>
@@ -8302,34 +8302,34 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>Ein Frankfurt</t>
+          <t>M'gladbach</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="G177" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H177" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I177" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J177" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K177" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L177" t="n">
-        <v>-0.1</v>
+        <v>-1.8</v>
       </c>
       <c r="M177" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="178">
@@ -8446,7 +8446,7 @@
         </is>
       </c>
       <c r="G180" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H180" t="n">
         <v>10</v>
@@ -8581,7 +8581,7 @@
         </is>
       </c>
       <c r="G183" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H183" t="n">
         <v>4</v>
@@ -8874,7 +8874,7 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B190" t="n">
         <v>18</v>
@@ -8887,39 +8887,39 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Hertha</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="G190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H190" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I190" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J190" t="n">
-        <v>7</v>
+        <v>-4</v>
       </c>
       <c r="K190" t="n">
-        <v>-7</v>
+        <v>4</v>
       </c>
       <c r="L190" t="n">
-        <v>-1.5</v>
+        <v>0.8</v>
       </c>
       <c r="M190" t="n">
-        <v>1.2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="B191" t="n">
         <v>18</v>
@@ -8932,34 +8932,34 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>Hertha</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="G191" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H191" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I191" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J191" t="n">
-        <v>-4</v>
+        <v>7</v>
       </c>
       <c r="K191" t="n">
-        <v>4</v>
+        <v>-7</v>
       </c>
       <c r="L191" t="n">
-        <v>0.8</v>
+        <v>-1.5</v>
       </c>
       <c r="M191" t="n">
-        <v>2.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="192">
@@ -9031,7 +9031,7 @@
         </is>
       </c>
       <c r="G193" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H193" t="n">
         <v>3</v>
@@ -9076,7 +9076,7 @@
         </is>
       </c>
       <c r="G194" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H194" t="n">
         <v>12</v>
@@ -9391,7 +9391,7 @@
         </is>
       </c>
       <c r="G201" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H201" t="n">
         <v>8</v>
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="G202" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H202" t="n">
         <v>4</v>
@@ -9860,7 +9860,7 @@
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B212" t="n">
         <v>27</v>
@@ -9873,39 +9873,39 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Fortuna Dusseldorf</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G212" t="n">
         <v>1</v>
       </c>
       <c r="H212" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I212" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J212" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K212" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="L212" t="n">
-        <v>-0.7</v>
+        <v>-0.2</v>
       </c>
       <c r="M212" t="n">
-        <v>1.1</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B213" t="n">
         <v>27</v>
@@ -9918,34 +9918,34 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>Fortuna Dusseldorf</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G213" t="n">
         <v>1</v>
       </c>
       <c r="H213" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I213" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J213" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K213" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="L213" t="n">
-        <v>-0.2</v>
+        <v>-0.7</v>
       </c>
       <c r="M213" t="n">
-        <v>1.4</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="214">
@@ -10017,7 +10017,7 @@
         </is>
       </c>
       <c r="G215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H215" t="n">
         <v>4</v>
@@ -10062,7 +10062,7 @@
         </is>
       </c>
       <c r="G216" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H216" t="n">
         <v>2</v>
@@ -10107,7 +10107,7 @@
         </is>
       </c>
       <c r="G217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H217" t="n">
         <v>3</v>
@@ -10240,7 +10240,7 @@
         </is>
       </c>
       <c r="G220" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H220" t="n">
         <v>8</v>
@@ -10375,7 +10375,7 @@
         </is>
       </c>
       <c r="G223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H223" t="n">
         <v>3</v>
@@ -10510,7 +10510,7 @@
         </is>
       </c>
       <c r="G226" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H226" t="n">
         <v>2</v>
@@ -10600,7 +10600,7 @@
         </is>
       </c>
       <c r="G228" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H228" t="n">
         <v>4</v>
@@ -10645,7 +10645,7 @@
         </is>
       </c>
       <c r="G229" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H229" t="n">
         <v>5</v>
@@ -10690,7 +10690,7 @@
         </is>
       </c>
       <c r="G230" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H230" t="n">
         <v>9</v>
@@ -10735,7 +10735,7 @@
         </is>
       </c>
       <c r="G231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H231" t="n">
         <v>13</v>
@@ -10868,7 +10868,7 @@
         </is>
       </c>
       <c r="G234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H234" t="n">
         <v>7</v>
@@ -11138,7 +11138,7 @@
         </is>
       </c>
       <c r="G240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H240" t="n">
         <v>7</v>
@@ -11361,7 +11361,7 @@
         </is>
       </c>
       <c r="G245" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H245" t="n">
         <v>4</v>
@@ -11406,7 +11406,7 @@
         </is>
       </c>
       <c r="G246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H246" t="n">
         <v>6</v>
@@ -11451,7 +11451,7 @@
         </is>
       </c>
       <c r="G247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H247" t="n">
         <v>14</v>
@@ -11586,7 +11586,7 @@
         </is>
       </c>
       <c r="G250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H250" t="n">
         <v>5</v>
@@ -11674,7 +11674,7 @@
         </is>
       </c>
       <c r="G252" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H252" t="n">
         <v>5</v>
@@ -11899,7 +11899,7 @@
         </is>
       </c>
       <c r="G257" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H257" t="n">
         <v>7</v>
@@ -11944,7 +11944,7 @@
         </is>
       </c>
       <c r="G258" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H258" t="n">
         <v>7</v>
@@ -11989,7 +11989,7 @@
         </is>
       </c>
       <c r="G259" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H259" t="n">
         <v>4</v>
@@ -12124,7 +12124,7 @@
         </is>
       </c>
       <c r="G262" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H262" t="n">
         <v>11</v>
@@ -12169,7 +12169,7 @@
         </is>
       </c>
       <c r="G263" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H263" t="n">
         <v>4</v>
@@ -12302,7 +12302,7 @@
         </is>
       </c>
       <c r="G266" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H266" t="n">
         <v>10</v>
@@ -12347,7 +12347,7 @@
         </is>
       </c>
       <c r="G267" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H267" t="n">
         <v>3</v>
@@ -12707,7 +12707,7 @@
         </is>
       </c>
       <c r="G275" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H275" t="n">
         <v>6</v>
@@ -13022,7 +13022,7 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H282" t="n">
         <v>4</v>
@@ -13067,7 +13067,7 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H283" t="n">
         <v>3</v>
@@ -13382,7 +13382,7 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H290" t="n">
         <v>7</v>
@@ -13470,7 +13470,7 @@
         </is>
       </c>
       <c r="G292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H292" t="n">
         <v>4</v>
@@ -13558,7 +13558,7 @@
         </is>
       </c>
       <c r="G294" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H294" t="n">
         <v>2</v>
@@ -13603,7 +13603,7 @@
         </is>
       </c>
       <c r="G295" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H295" t="n">
         <v>3</v>
@@ -13716,7 +13716,7 @@
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B298" t="n">
         <v>16</v>
@@ -13729,12 +13729,12 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Schalke 04</t>
+          <t>Hertha</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G298" t="n">
@@ -13744,7 +13744,7 @@
         <v>2</v>
       </c>
       <c r="I298" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J298" t="n">
         <v>0</v>
@@ -13753,15 +13753,15 @@
         <v>0</v>
       </c>
       <c r="L298" t="n">
-        <v>-0.8</v>
+        <v>0.2</v>
       </c>
       <c r="M298" t="n">
-        <v>1.1</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B299" t="n">
         <v>16</v>
@@ -13774,12 +13774,12 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Hertha</t>
+          <t>Schalke 04</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G299" t="n">
@@ -13789,7 +13789,7 @@
         <v>2</v>
       </c>
       <c r="I299" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J299" t="n">
         <v>0</v>
@@ -13798,10 +13798,10 @@
         <v>0</v>
       </c>
       <c r="L299" t="n">
-        <v>0.2</v>
+        <v>-0.8</v>
       </c>
       <c r="M299" t="n">
-        <v>1.6</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="300">
@@ -13963,7 +13963,7 @@
         </is>
       </c>
       <c r="G303" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H303" t="n">
         <v>4</v>
@@ -14098,7 +14098,7 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H306" t="n">
         <v>8</v>
@@ -14458,7 +14458,7 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H314" t="n">
         <v>2</v>
@@ -14548,7 +14548,7 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H316" t="n">
         <v>2</v>
@@ -14816,7 +14816,7 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H322" t="n">
         <v>1</v>
@@ -14906,7 +14906,7 @@
         </is>
       </c>
       <c r="G324" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H324" t="n">
         <v>4</v>
@@ -15039,7 +15039,7 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H327" t="n">
         <v>5</v>
@@ -15217,7 +15217,7 @@
         </is>
       </c>
       <c r="G331" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H331" t="n">
         <v>6</v>
@@ -15285,7 +15285,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B333" t="n">
         <v>26</v>
@@ -15298,39 +15298,39 @@
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>M'gladbach</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="G333" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H333" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I333" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J333" t="n">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="K333" t="n">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="L333" t="n">
-        <v>-0.5</v>
+        <v>0.1</v>
       </c>
       <c r="M333" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B334" t="n">
         <v>26</v>
@@ -15343,34 +15343,34 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>M'gladbach</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="G334" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H334" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I334" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J334" t="n">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="K334" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="L334" t="n">
-        <v>0.1</v>
+        <v>-0.5</v>
       </c>
       <c r="M334" t="n">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="335">
@@ -15639,7 +15639,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B341" t="n">
         <v>19</v>
@@ -15652,39 +15652,39 @@
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>Ein Frankfurt</t>
+          <t>Hannover</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G341" t="n">
         <v>1</v>
       </c>
       <c r="H341" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I341" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J341" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="K341" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="L341" t="n">
-        <v>-1</v>
+        <v>0.2</v>
       </c>
       <c r="M341" t="n">
-        <v>1.1</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B342" t="n">
         <v>19</v>
@@ -15697,34 +15697,34 @@
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>Hannover</t>
+          <t>Ein Frankfurt</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G342" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H342" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I342" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J342" t="n">
+        <v>2</v>
+      </c>
+      <c r="K342" t="n">
+        <v>-2</v>
+      </c>
+      <c r="L342" t="n">
         <v>-1</v>
       </c>
-      <c r="K342" t="n">
-        <v>1</v>
-      </c>
-      <c r="L342" t="n">
-        <v>0.2</v>
-      </c>
       <c r="M342" t="n">
-        <v>1.7</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="343">
@@ -15796,7 +15796,7 @@
         </is>
       </c>
       <c r="G344" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H344" t="n">
         <v>5</v>
@@ -15841,7 +15841,7 @@
         </is>
       </c>
       <c r="G345" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H345" t="n">
         <v>8</v>
@@ -15929,7 +15929,7 @@
         </is>
       </c>
       <c r="G347" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H347" t="n">
         <v>5</v>
@@ -15952,7 +15952,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B348" t="n">
         <v>12</v>
@@ -15965,28 +15965,28 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>M'gladbach</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G348" t="n">
         <v>1</v>
       </c>
       <c r="H348" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I348" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J348" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="K348" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="L348" t="n">
         <v>0</v>
@@ -15995,7 +15995,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B349" t="n">
         <v>12</v>
@@ -16008,28 +16008,28 @@
       </c>
       <c r="E349" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>M'gladbach</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G349" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H349" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I349" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J349" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="K349" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="L349" t="n">
         <v>0</v>
@@ -16060,7 +16060,7 @@
         </is>
       </c>
       <c r="G350" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H350" t="n">
         <v>7</v>
@@ -16369,7 +16369,7 @@
         </is>
       </c>
       <c r="G357" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H357" t="n">
         <v>4</v>
@@ -16476,7 +16476,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B360" t="n">
         <v>22</v>
@@ -16489,28 +16489,28 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>Nurnberg</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G360" t="n">
         <v>1</v>
       </c>
       <c r="H360" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I360" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J360" t="n">
+        <v>1</v>
+      </c>
+      <c r="K360" t="n">
         <v>-1</v>
-      </c>
-      <c r="K360" t="n">
-        <v>1</v>
       </c>
       <c r="L360" t="n">
         <v>0</v>
@@ -16519,7 +16519,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="n">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B361" t="n">
         <v>22</v>
@@ -16532,28 +16532,28 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Nurnberg</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G361" t="n">
         <v>1</v>
       </c>
       <c r="H361" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I361" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J361" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K361" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L361" t="n">
         <v>0</v>
@@ -16885,7 +16885,7 @@
         </is>
       </c>
       <c r="G369" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H369" t="n">
         <v>4</v>
@@ -17272,7 +17272,7 @@
         </is>
       </c>
       <c r="G378" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H378" t="n">
         <v>7</v>
@@ -17336,7 +17336,7 @@
     </row>
     <row r="380">
       <c r="A380" s="1" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B380" t="n">
         <v>15</v>
@@ -17349,28 +17349,28 @@
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>Fortuna Dusseldorf</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G380" t="n">
         <v>1</v>
       </c>
       <c r="H380" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I380" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J380" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K380" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="L380" t="n">
         <v>0</v>
@@ -17379,7 +17379,7 @@
     </row>
     <row r="381">
       <c r="A381" s="1" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B381" t="n">
         <v>15</v>
@@ -17392,28 +17392,28 @@
       </c>
       <c r="E381" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Fortuna Dusseldorf</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G381" t="n">
         <v>1</v>
       </c>
       <c r="H381" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I381" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J381" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K381" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="L381" t="n">
         <v>0</v>
@@ -17745,7 +17745,7 @@
         </is>
       </c>
       <c r="G389" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H389" t="n">
         <v>7</v>
@@ -17919,7 +17919,7 @@
         </is>
       </c>
       <c r="G393" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H393" t="n">
         <v>5</v>
@@ -18091,7 +18091,7 @@
         </is>
       </c>
       <c r="G397" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H397" t="n">
         <v>3</v>
@@ -18521,7 +18521,7 @@
         </is>
       </c>
       <c r="G407" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H407" t="n">
         <v>6</v>
@@ -18779,7 +18779,7 @@
         </is>
       </c>
       <c r="G413" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H413" t="n">
         <v>1</v>
@@ -19209,7 +19209,7 @@
         </is>
       </c>
       <c r="G423" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H423" t="n">
         <v>5</v>
@@ -19295,7 +19295,7 @@
         </is>
       </c>
       <c r="G425" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H425" t="n">
         <v>1</v>
@@ -19381,7 +19381,7 @@
         </is>
       </c>
       <c r="G427" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H427" t="n">
         <v>2</v>
@@ -20241,7 +20241,7 @@
         </is>
       </c>
       <c r="G447" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H447" t="n">
         <v>2</v>
@@ -20993,7 +20993,7 @@
     </row>
     <row r="465">
       <c r="A465" s="1" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B465" t="n">
         <v>22</v>
@@ -21006,28 +21006,28 @@
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="F465" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G465" t="n">
         <v>1</v>
       </c>
       <c r="H465" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I465" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J465" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="K465" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L465" t="n">
         <v>0</v>
@@ -21036,7 +21036,7 @@
     </row>
     <row r="466">
       <c r="A466" s="1" t="n">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B466" t="n">
         <v>22</v>
@@ -21049,28 +21049,28 @@
       </c>
       <c r="E466" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="F466" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G466" t="n">
         <v>1</v>
       </c>
       <c r="H466" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I466" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J466" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="K466" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L466" t="n">
         <v>0</v>
@@ -21359,7 +21359,7 @@
         </is>
       </c>
       <c r="G473" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H473" t="n">
         <v>8</v>
@@ -21509,7 +21509,7 @@
     </row>
     <row r="477">
       <c r="A477" s="1" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B477" t="n">
         <v>15</v>
@@ -21522,28 +21522,28 @@
       </c>
       <c r="E477" t="inlineStr">
         <is>
-          <t>Mainz</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="F477" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="G477" t="n">
         <v>1</v>
       </c>
       <c r="H477" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I477" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J477" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K477" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="L477" t="n">
         <v>0</v>
@@ -21552,7 +21552,7 @@
     </row>
     <row r="478">
       <c r="A478" s="1" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B478" t="n">
         <v>15</v>
@@ -21565,28 +21565,28 @@
       </c>
       <c r="E478" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>Mainz</t>
         </is>
       </c>
       <c r="F478" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="G478" t="n">
         <v>1</v>
       </c>
       <c r="H478" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I478" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J478" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K478" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="L478" t="n">
         <v>0</v>
@@ -22176,7 +22176,7 @@
         </is>
       </c>
       <c r="G492" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H492" t="n">
         <v>5</v>
@@ -22326,7 +22326,7 @@
     </row>
     <row r="496">
       <c r="A496" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B496" t="n">
         <v>25</v>
@@ -22339,28 +22339,28 @@
       </c>
       <c r="E496" t="inlineStr">
         <is>
-          <t>Fortuna Dusseldorf</t>
+          <t>M'gladbach</t>
         </is>
       </c>
       <c r="F496" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="G496" t="n">
         <v>1</v>
       </c>
       <c r="H496" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I496" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J496" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="K496" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="L496" t="n">
         <v>0</v>
@@ -22369,7 +22369,7 @@
     </row>
     <row r="497">
       <c r="A497" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B497" t="n">
         <v>25</v>
@@ -22382,28 +22382,28 @@
       </c>
       <c r="E497" t="inlineStr">
         <is>
-          <t>M'gladbach</t>
+          <t>Fortuna Dusseldorf</t>
         </is>
       </c>
       <c r="F497" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="G497" t="n">
         <v>1</v>
       </c>
       <c r="H497" t="n">
+        <v>5</v>
+      </c>
+      <c r="I497" t="n">
         <v>7</v>
       </c>
-      <c r="I497" t="n">
-        <v>3</v>
-      </c>
       <c r="J497" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="K497" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="L497" t="n">
         <v>0</v>
@@ -23079,7 +23079,7 @@
         </is>
       </c>
       <c r="G513" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H513" t="n">
         <v>5</v>
@@ -23939,7 +23939,7 @@
         </is>
       </c>
       <c r="G533" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H533" t="n">
         <v>2</v>
@@ -24627,7 +24627,7 @@
         </is>
       </c>
       <c r="G549" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H549" t="n">
         <v>3</v>
@@ -24713,7 +24713,7 @@
         </is>
       </c>
       <c r="G551" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H551" t="n">
         <v>2</v>
@@ -24799,7 +24799,7 @@
         </is>
       </c>
       <c r="G553" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H553" t="n">
         <v>7</v>
@@ -24842,7 +24842,7 @@
         </is>
       </c>
       <c r="G554" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H554" t="n">
         <v>3</v>
@@ -24885,7 +24885,7 @@
         </is>
       </c>
       <c r="G555" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H555" t="n">
         <v>10</v>
@@ -24928,7 +24928,7 @@
         </is>
       </c>
       <c r="G556" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H556" t="n">
         <v>2</v>
@@ -24971,7 +24971,7 @@
         </is>
       </c>
       <c r="G557" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H557" t="n">
         <v>3</v>
@@ -24992,7 +24992,7 @@
     </row>
     <row r="558">
       <c r="A558" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B558" t="n">
         <v>9</v>
@@ -25005,28 +25005,28 @@
       </c>
       <c r="E558" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Ein Frankfurt</t>
         </is>
       </c>
       <c r="F558" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G558" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H558" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I558" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J558" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="K558" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="L558" t="n">
         <v>0</v>
@@ -25035,7 +25035,7 @@
     </row>
     <row r="559">
       <c r="A559" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B559" t="n">
         <v>9</v>
@@ -25048,28 +25048,28 @@
       </c>
       <c r="E559" t="inlineStr">
         <is>
-          <t>Ein Frankfurt</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="F559" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G559" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H559" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I559" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J559" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="K559" t="n">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="L559" t="n">
         <v>0</v>
@@ -25100,7 +25100,7 @@
         </is>
       </c>
       <c r="G560" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H560" t="n">
         <v>7</v>
@@ -25143,7 +25143,7 @@
         </is>
       </c>
       <c r="G561" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H561" t="n">
         <v>0</v>
@@ -25186,7 +25186,7 @@
         </is>
       </c>
       <c r="G562" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H562" t="n">
         <v>4</v>

</xml_diff>